<commit_message>
Made the USB Mapping document more cohesive
</commit_message>
<xml_diff>
--- a/Extra/USBMAP.xlsx
+++ b/Extra/USBMAP.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dmnerd/Documents/GitHub/Hackintosh/Extra/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA355FC-19C8-CF45-A546-D0290E15BBB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0E20B1-18E9-E249-85B8-942144774733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{8DC37123-26A2-A44B-9019-488C203901E7}"/>
+    <workbookView xWindow="1120" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{8DC37123-26A2-A44B-9019-488C203901E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="SS02_">Sheet1!$B$2</definedName>
+    <definedName name="SS02_">Sheet1!$F$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="34">
   <si>
     <t>HS04</t>
   </si>
@@ -125,6 +125,21 @@
   </si>
   <si>
     <t>Internal</t>
+  </si>
+  <si>
+    <t>1, 2</t>
+  </si>
+  <si>
+    <t>3, 4</t>
+  </si>
+  <si>
+    <t>5, 6</t>
+  </si>
+  <si>
+    <t>Back Panel</t>
+  </si>
+  <si>
+    <t>Internal (Front panel connections)</t>
   </si>
 </sst>
 </file>
@@ -204,7 +219,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -343,6 +358,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -351,14 +375,14 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -370,6 +394,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -389,6 +414,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BF1B7AF-274A-6F38-15A2-40426A10269B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="787400" y="177800"/>
+          <a:ext cx="1841500" cy="5562600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -688,330 +762,367 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12613A11-F187-0F49-BCD3-2104D1DD0925}">
-  <dimension ref="B1:H24"/>
+  <dimension ref="A2:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:H24"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="E2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+    <row r="5" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E6" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="E5" s="3" t="s">
+    <row r="7" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="I7" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+    <row r="8" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+    <row r="9" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
+    <row r="10" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F11" t="s">
         <v>15</v>
       </c>
-      <c r="C9">
-        <f>COUNTA(B2:C7)</f>
+      <c r="G11">
+        <f>COUNTA(F4:G9)</f>
         <v>10</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="I11" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="J11" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="K11" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="L11" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F12" t="s">
         <v>16</v>
       </c>
-      <c r="C10">
-        <f>COUNTA(E2:H3)</f>
+      <c r="G12">
+        <f>COUNTA(I4:L5)</f>
         <v>4</v>
       </c>
-      <c r="E10" s="15">
+      <c r="I12" s="15">
         <v>1</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="J12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="K12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="L12" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="13" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" t="s">
         <v>17</v>
       </c>
-      <c r="C11">
+      <c r="G13">
         <v>1</v>
       </c>
-      <c r="E11" s="16">
+      <c r="I13" s="16">
         <v>2</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="J13" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="K13" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="L13" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+    <row r="14" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
         <v>18</v>
       </c>
-      <c r="C12">
-        <f>SUM(C9:C11)</f>
+      <c r="G14">
+        <f>SUM(G11:G13)</f>
         <v>15</v>
       </c>
-      <c r="E12" s="16">
+      <c r="I14" s="16">
         <v>3</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="J14" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="K14" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="L14" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E13" s="16">
+    <row r="15" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I15" s="16">
         <v>4</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="J15" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="K15" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="L15" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="E14" s="16">
+    <row r="16" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="I16" s="16">
         <v>5</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="J16" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="K16" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="L16" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E15" s="16">
+    <row r="17" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I17" s="16">
         <v>6</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="J17" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="K17" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H15" s="7" t="s">
+      <c r="L17" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E16" s="16">
+    <row r="18" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I18" s="16">
         <v>7</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="J18" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="K18" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H16" s="7" t="s">
+      <c r="L18" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="5:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E17" s="16">
+    <row r="19" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I19" s="16">
         <v>8</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="J19" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="K19" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H17" s="7" t="s">
+      <c r="L19" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="5:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="E18" s="16">
+    <row r="20" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="I20" s="16">
         <v>9</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="J20" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="K20" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H18" s="7" t="s">
+      <c r="L20" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E19" s="16">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I21" s="16">
         <v>10</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="J21" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="K21" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H19" s="7" t="s">
+      <c r="L21" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E20" s="16">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="I22" s="16">
         <v>11</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="J22" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="K22" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H20" s="7" t="s">
+      <c r="L22" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="5:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E21" s="16">
+    <row r="23" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I23" s="16">
         <v>12</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="J23" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="K23" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H21" s="7" t="s">
+      <c r="L23" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="5:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E22" s="16">
+    <row r="24" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I24" s="16">
         <v>13</v>
       </c>
-      <c r="F22" s="14" t="s">
+      <c r="J24" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="G22" s="6" t="s">
+      <c r="K24" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H22" s="7" t="s">
+      <c r="L24" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="5:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E23" s="16">
+    <row r="25" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I25" s="16">
         <v>14</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="J25" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G23" s="6" t="s">
+      <c r="K25" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H23" s="7" t="s">
+      <c r="L25" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="5:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E24" s="17">
+    <row r="26" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I26" s="17">
         <v>15</v>
       </c>
-      <c r="F24" s="8" t="s">
+      <c r="J26" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G24" s="9" t="s">
+      <c r="K26" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="H24" s="10" t="s">
+      <c r="L26" s="10" t="s">
         <v>28</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>